<commit_message>
some updates on the texts.
</commit_message>
<xml_diff>
--- a/NetworkConfigData/ModalConfig_NETS_NYPS_68bus_detuned_gov_FS.xlsx
+++ b/NetworkConfigData/ModalConfig_NETS_NYPS_68bus_detuned_gov_FS.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Git\Publications\GreyBoxApproach\Model\NetworkConfigData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Git\Simplex-Power-Systems\NetworkConfigData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4D4A2F-CC42-442B-95B3-3487C49646F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75BC5C7-6D4F-4D49-9FBD-7BA0D63FBB42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2055" yWindow="2385" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{83EB2F79-8531-4BD7-80A7-107967E163E3}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{83EB2F79-8531-4BD7-80A7-107967E163E3}"/>
   </bookViews>
   <sheets>
-    <sheet name="State-PF" sheetId="18" r:id="rId1"/>
-    <sheet name="Impedance-PF" sheetId="19" r:id="rId2"/>
-    <sheet name="Enabling" sheetId="20" r:id="rId3"/>
+    <sheet name="State-PF" sheetId="21" r:id="rId1"/>
+    <sheet name="Impedance-PF" sheetId="22" r:id="rId2"/>
+    <sheet name="Enabling" sheetId="23" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -6919,7 +6919,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61BB00C5-0415-480E-87DD-B091A9D58F6B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F1C13FA-B22D-4E1D-8ABA-9B2DC02AD7A9}">
   <dimension ref="A1:G1197"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -27280,11 +27280,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF7A86C-09E7-4996-AEDB-72D1B69F7B9A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC41C2FC-F2C3-460D-A70C-6400C123CE64}">
   <dimension ref="A1:L1198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27353,7 +27353,7 @@
         <v>2168</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" t="s">
         <v>9</v>
@@ -27708,7 +27708,7 @@
         <v>563</v>
       </c>
       <c r="L22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -27800,7 +27800,7 @@
         <v>681</v>
       </c>
       <c r="L26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -27823,7 +27823,7 @@
         <v>695</v>
       </c>
       <c r="L27">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -31169,7 +31169,7 @@
         <v>664</v>
       </c>
       <c r="I329">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="330" spans="7:9" x14ac:dyDescent="0.25">
@@ -31653,7 +31653,7 @@
         <v>742</v>
       </c>
       <c r="I373">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="374" spans="7:9" x14ac:dyDescent="0.25">
@@ -40737,11 +40737,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{793D596F-0252-40C4-951B-841B1349E095}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E9169D-6321-4296-B9BC-F372CD8F7A87}">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40777,7 +40777,7 @@
         <v>2175</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>